<commit_message>
Update Medicare SAPTO 2003-04
</commit_message>
<xml_diff>
--- a/data-raw/SAPTO-rates.xlsx
+++ b/data-raw/SAPTO-rates.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GitHub\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Parsonage\Documents\Github\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,6 +253,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -288,6 +305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -490,7 +524,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -522,7 +556,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -557,19 +591,19 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E4">
-        <v>31279</v>
+        <v>32279</v>
       </c>
       <c r="F4">
-        <v>95198</v>
+        <v>50119</v>
       </c>
       <c r="G4">
         <v>0.125</v>
@@ -586,22 +620,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E5">
-        <v>32279</v>
+        <v>28974</v>
       </c>
       <c r="F5">
-        <v>50119</v>
+        <v>83580</v>
       </c>
       <c r="G5">
         <v>0.125</v>
@@ -618,22 +652,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>1602</v>
+        <v>2040</v>
       </c>
       <c r="E6">
-        <v>28974</v>
+        <v>31279</v>
       </c>
       <c r="F6">
-        <v>83580</v>
+        <v>95198</v>
       </c>
       <c r="G6">
         <v>0.125</v>
@@ -653,19 +687,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E7">
-        <v>31279</v>
+        <v>32279</v>
       </c>
       <c r="F7">
-        <v>95198</v>
+        <v>50119</v>
       </c>
       <c r="G7">
         <v>0.125</v>
@@ -682,22 +716,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E8">
-        <v>32279</v>
+        <v>28974</v>
       </c>
       <c r="F8">
-        <v>50119</v>
+        <v>83580</v>
       </c>
       <c r="G8">
         <v>0.125</v>
@@ -714,22 +748,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>1602</v>
+        <v>2040</v>
       </c>
       <c r="E9">
-        <v>28974</v>
+        <v>31279</v>
       </c>
       <c r="F9">
-        <v>83580</v>
+        <v>95198</v>
       </c>
       <c r="G9">
         <v>0.125</v>
@@ -749,19 +783,19 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E10">
-        <v>31279</v>
+        <v>32279</v>
       </c>
       <c r="F10">
-        <v>95198</v>
+        <v>50119</v>
       </c>
       <c r="G10">
         <v>0.125</v>
@@ -778,22 +812,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E11">
-        <v>32279</v>
+        <v>28974</v>
       </c>
       <c r="F11">
-        <v>50119</v>
+        <v>83580</v>
       </c>
       <c r="G11">
         <v>0.125</v>
@@ -810,22 +844,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>1602</v>
+        <v>2040</v>
       </c>
       <c r="E12">
-        <v>28974</v>
+        <v>31279</v>
       </c>
       <c r="F12">
-        <v>83580</v>
+        <v>95198</v>
       </c>
       <c r="G12">
         <v>0.125</v>
@@ -845,19 +879,19 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E13">
-        <v>31279</v>
+        <v>32279</v>
       </c>
       <c r="F13">
-        <v>95198</v>
+        <v>50119</v>
       </c>
       <c r="G13">
         <v>0.125</v>
@@ -874,31 +908,31 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E14">
-        <v>24867</v>
+        <v>28974</v>
       </c>
       <c r="F14">
-        <v>42707</v>
+        <v>83580</v>
       </c>
       <c r="G14">
         <v>0.125</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="b">
         <v>0</v>
@@ -906,34 +940,31 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>1602</v>
+        <v>2040</v>
       </c>
       <c r="E15">
-        <v>21680</v>
+        <v>31279</v>
       </c>
       <c r="F15">
-        <v>66992</v>
+        <v>95198</v>
       </c>
       <c r="G15">
         <v>0.125</v>
       </c>
-      <c r="H15" t="s">
-        <v>25</v>
-      </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
@@ -941,28 +972,28 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E16">
-        <v>23600</v>
+        <v>30685</v>
       </c>
       <c r="F16">
-        <v>79840</v>
+        <v>48525</v>
       </c>
       <c r="G16">
         <v>0.125</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -976,7 +1007,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -985,103 +1016,103 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>2018</v>
+        <v>2230</v>
       </c>
       <c r="E17">
-        <v>19454</v>
+        <v>30685</v>
       </c>
       <c r="F17">
-        <v>71196</v>
+        <v>48525</v>
       </c>
       <c r="G17">
         <v>0.125</v>
       </c>
       <c r="H17" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>1522</v>
+        <v>2230</v>
       </c>
       <c r="E18">
-        <v>16147</v>
+        <v>29867</v>
       </c>
       <c r="F18">
-        <v>56646</v>
+        <v>47707</v>
       </c>
       <c r="G18">
         <v>0.125</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>1879</v>
+        <v>2230</v>
       </c>
       <c r="E19">
-        <v>18257</v>
+        <v>28867</v>
       </c>
       <c r="F19">
-        <v>67118</v>
+        <v>46707</v>
       </c>
       <c r="G19">
         <v>0.125</v>
       </c>
       <c r="H19" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1090,33 +1121,33 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <v>2230</v>
+        <v>2018</v>
       </c>
       <c r="E20">
-        <v>21968</v>
+        <v>19454</v>
       </c>
       <c r="F20">
-        <v>39808</v>
+        <v>71196</v>
       </c>
       <c r="G20">
         <v>0.125</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1125,33 +1156,33 @@
         <v>6</v>
       </c>
       <c r="D21">
-        <v>1602</v>
+        <v>1522</v>
       </c>
       <c r="E21">
-        <v>18247</v>
+        <v>16147</v>
       </c>
       <c r="F21">
-        <v>31063</v>
+        <v>56646</v>
       </c>
       <c r="G21">
         <v>0.125</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
       </c>
       <c r="J21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1160,33 +1191,33 @@
         <v>9</v>
       </c>
       <c r="D22">
-        <v>2040</v>
+        <v>1879</v>
       </c>
       <c r="E22">
-        <v>21167</v>
+        <v>18257</v>
       </c>
       <c r="F22">
-        <v>37487</v>
+        <v>67118</v>
       </c>
       <c r="G22">
         <v>0.125</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1195,33 +1226,33 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>1928</v>
+        <v>2230</v>
       </c>
       <c r="E23">
-        <v>17342</v>
+        <v>24867</v>
       </c>
       <c r="F23">
-        <v>32766</v>
+        <v>42707</v>
       </c>
       <c r="G23">
         <v>0.125</v>
       </c>
       <c r="H23" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1230,33 +1261,33 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <v>1424</v>
+        <v>1602</v>
       </c>
       <c r="E24">
-        <v>14377</v>
+        <v>20680</v>
       </c>
       <c r="F24">
-        <v>25769</v>
+        <v>66992</v>
       </c>
       <c r="G24">
         <v>0.125</v>
       </c>
       <c r="H24" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1265,33 +1296,33 @@
         <v>9</v>
       </c>
       <c r="D25">
-        <v>1782</v>
+        <v>2040</v>
       </c>
       <c r="E25">
-        <v>16483</v>
+        <v>23600</v>
       </c>
       <c r="F25">
-        <v>30739</v>
+        <v>79840</v>
       </c>
       <c r="G25">
         <v>0.125</v>
       </c>
       <c r="H25" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1300,33 +1331,33 @@
         <v>4</v>
       </c>
       <c r="D26">
-        <v>2230</v>
+        <v>2018</v>
       </c>
       <c r="E26">
-        <v>20500</v>
+        <v>19454</v>
       </c>
       <c r="F26">
-        <v>38340</v>
+        <v>71196</v>
       </c>
       <c r="G26">
         <v>0.125</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1335,33 +1366,33 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>1602</v>
+        <v>1522</v>
       </c>
       <c r="E27">
-        <v>16806</v>
+        <v>16147</v>
       </c>
       <c r="F27">
-        <v>29622</v>
+        <v>56646</v>
       </c>
       <c r="G27">
         <v>0.125</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1370,33 +1401,33 @@
         <v>9</v>
       </c>
       <c r="D28">
-        <v>2040</v>
+        <v>1879</v>
       </c>
       <c r="E28">
-        <v>19383</v>
+        <v>18257</v>
       </c>
       <c r="F28">
-        <v>35703</v>
+        <v>67118</v>
       </c>
       <c r="G28">
         <v>0.125</v>
       </c>
       <c r="H28" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1405,33 +1436,30 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>1928</v>
+        <v>2230</v>
       </c>
       <c r="E29">
-        <v>17342</v>
+        <v>24867</v>
       </c>
       <c r="F29">
-        <v>32766</v>
+        <v>42707</v>
       </c>
       <c r="G29">
         <v>0.125</v>
       </c>
-      <c r="H29" t="s">
-        <v>19</v>
-      </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1440,33 +1468,33 @@
         <v>6</v>
       </c>
       <c r="D30">
-        <v>1424</v>
+        <v>1602</v>
       </c>
       <c r="E30">
-        <v>14377</v>
+        <v>21680</v>
       </c>
       <c r="F30">
-        <v>25769</v>
+        <v>66992</v>
       </c>
       <c r="G30">
         <v>0.125</v>
       </c>
       <c r="H30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -1475,33 +1503,33 @@
         <v>9</v>
       </c>
       <c r="D31">
-        <v>1782</v>
+        <v>2040</v>
       </c>
       <c r="E31">
-        <v>16483</v>
+        <v>23600</v>
       </c>
       <c r="F31">
-        <v>30739</v>
+        <v>79840</v>
       </c>
       <c r="G31">
         <v>0.125</v>
       </c>
       <c r="H31" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1510,33 +1538,33 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>2230</v>
+        <v>1928</v>
       </c>
       <c r="E32">
-        <v>20500</v>
+        <v>17342</v>
       </c>
       <c r="F32">
-        <v>38340</v>
+        <v>32766</v>
       </c>
       <c r="G32">
         <v>0.125</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1545,33 +1573,33 @@
         <v>6</v>
       </c>
       <c r="D33">
-        <v>1602</v>
+        <v>1424</v>
       </c>
       <c r="E33">
-        <v>16806</v>
+        <v>14377</v>
       </c>
       <c r="F33">
-        <v>29622</v>
+        <v>25769</v>
       </c>
       <c r="G33">
         <v>0.125</v>
       </c>
       <c r="H33" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1580,33 +1608,33 @@
         <v>9</v>
       </c>
       <c r="D34">
-        <v>2040</v>
+        <v>1782</v>
       </c>
       <c r="E34">
-        <v>19383</v>
+        <v>16483</v>
       </c>
       <c r="F34">
-        <v>35703</v>
+        <v>30739</v>
       </c>
       <c r="G34">
         <v>0.125</v>
       </c>
       <c r="H34" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
       </c>
       <c r="J34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1615,33 +1643,33 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <v>1928</v>
+        <v>2230</v>
       </c>
       <c r="E35">
-        <v>17342</v>
+        <v>21968</v>
       </c>
       <c r="F35">
-        <v>32766</v>
+        <v>39808</v>
       </c>
       <c r="G35">
         <v>0.125</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1650,33 +1678,33 @@
         <v>6</v>
       </c>
       <c r="D36">
-        <v>1424</v>
+        <v>1602</v>
       </c>
       <c r="E36">
-        <v>14377</v>
+        <v>18247</v>
       </c>
       <c r="F36">
-        <v>25769</v>
+        <v>31063</v>
       </c>
       <c r="G36">
         <v>0.125</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -1685,33 +1713,33 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <v>1782</v>
+        <v>2040</v>
       </c>
       <c r="E37">
-        <v>16483</v>
+        <v>21167</v>
       </c>
       <c r="F37">
-        <v>30739</v>
+        <v>37487</v>
       </c>
       <c r="G37">
         <v>0.125</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
       </c>
       <c r="J37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1720,33 +1748,33 @@
         <v>4</v>
       </c>
       <c r="D38">
-        <v>2230</v>
+        <v>1928</v>
       </c>
       <c r="E38">
-        <v>24867</v>
+        <v>17342</v>
       </c>
       <c r="F38">
-        <v>42707</v>
+        <v>32766</v>
       </c>
       <c r="G38">
         <v>0.125</v>
       </c>
       <c r="H38" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1755,33 +1783,33 @@
         <v>6</v>
       </c>
       <c r="D39">
-        <v>1602</v>
+        <v>1424</v>
       </c>
       <c r="E39">
-        <v>20680</v>
+        <v>14377</v>
       </c>
       <c r="F39">
-        <v>66992</v>
+        <v>25769</v>
       </c>
       <c r="G39">
         <v>0.125</v>
       </c>
       <c r="H39" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1790,33 +1818,33 @@
         <v>9</v>
       </c>
       <c r="D40">
-        <v>2040</v>
+        <v>1782</v>
       </c>
       <c r="E40">
-        <v>23600</v>
+        <v>16483</v>
       </c>
       <c r="F40">
-        <v>79840</v>
+        <v>30739</v>
       </c>
       <c r="G40">
         <v>0.125</v>
       </c>
       <c r="H40" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1825,33 +1853,33 @@
         <v>4</v>
       </c>
       <c r="D41">
-        <v>2018</v>
+        <v>2230</v>
       </c>
       <c r="E41">
-        <v>19454</v>
+        <v>20500</v>
       </c>
       <c r="F41">
-        <v>71196</v>
+        <v>38340</v>
       </c>
       <c r="G41">
         <v>0.125</v>
       </c>
       <c r="H41" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
       </c>
       <c r="J41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -1860,33 +1888,33 @@
         <v>6</v>
       </c>
       <c r="D42">
-        <v>1522</v>
+        <v>1602</v>
       </c>
       <c r="E42">
-        <v>16147</v>
+        <v>16806</v>
       </c>
       <c r="F42">
-        <v>56646</v>
+        <v>29622</v>
       </c>
       <c r="G42">
         <v>0.125</v>
       </c>
       <c r="H42" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -1895,33 +1923,33 @@
         <v>9</v>
       </c>
       <c r="D43">
-        <v>1879</v>
+        <v>2040</v>
       </c>
       <c r="E43">
-        <v>18257</v>
+        <v>19383</v>
       </c>
       <c r="F43">
-        <v>67118</v>
+        <v>35703</v>
       </c>
       <c r="G43">
         <v>0.125</v>
       </c>
       <c r="H43" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1930,103 +1958,103 @@
         <v>4</v>
       </c>
       <c r="D44">
-        <v>2230</v>
+        <v>1928</v>
       </c>
       <c r="E44">
-        <v>28867</v>
+        <v>17342</v>
       </c>
       <c r="F44">
-        <v>46707</v>
+        <v>32766</v>
       </c>
       <c r="G44">
         <v>0.125</v>
       </c>
       <c r="H44" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D45">
-        <v>2230</v>
+        <v>1424</v>
       </c>
       <c r="E45">
-        <v>29867</v>
+        <v>14377</v>
       </c>
       <c r="F45">
-        <v>47707</v>
+        <v>25769</v>
       </c>
       <c r="G45">
         <v>0.125</v>
       </c>
       <c r="H45" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D46">
-        <v>2230</v>
+        <v>1782</v>
       </c>
       <c r="E46">
-        <v>30685</v>
+        <v>16483</v>
       </c>
       <c r="F46">
-        <v>48525</v>
+        <v>30739</v>
       </c>
       <c r="G46">
         <v>0.125</v>
       </c>
       <c r="H46" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I46" t="b">
         <v>0</v>
       </c>
       <c r="J46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2038,16 +2066,16 @@
         <v>2230</v>
       </c>
       <c r="E47">
-        <v>30685</v>
+        <v>20500</v>
       </c>
       <c r="F47">
-        <v>48525</v>
+        <v>38340</v>
       </c>
       <c r="G47">
         <v>0.125</v>
       </c>
       <c r="H47" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
@@ -2061,31 +2089,34 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E48">
-        <v>32279</v>
+        <v>16806</v>
       </c>
       <c r="F48">
-        <v>50119</v>
+        <v>29622</v>
       </c>
       <c r="G48">
         <v>0.125</v>
       </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
       <c r="I48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" t="b">
         <v>0</v>
@@ -2093,40 +2124,44 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D49">
-        <v>1602</v>
+        <v>2040</v>
       </c>
       <c r="E49">
-        <v>28974</v>
+        <v>19383</v>
       </c>
       <c r="F49">
-        <v>83580</v>
+        <v>35703</v>
       </c>
       <c r="G49">
         <v>0.125</v>
       </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
       <c r="I49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K31">
-    <sortCondition descending="1" ref="A2:A31"/>
-    <sortCondition descending="1" ref="J2:J31"/>
+  <sortState ref="A2:K49">
+    <sortCondition descending="1" ref="A2:A49"/>
+    <sortCondition ref="I2:I49"/>
+    <sortCondition ref="J2:J49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update SAPTO (keep legislated assumption)
</commit_message>
<xml_diff>
--- a/data-raw/SAPTO-rates.xlsx
+++ b/data-raw/SAPTO-rates.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Parsonage\Documents\Github\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughp\Documents\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="40">
   <si>
     <t>fy_year</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>2000-01</t>
+  </si>
+  <si>
+    <t>2017-18</t>
+  </si>
+  <si>
+    <t>2018-19</t>
+  </si>
+  <si>
+    <t>2019-20</t>
   </si>
 </sst>
 </file>
@@ -486,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +545,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -568,7 +577,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -600,7 +609,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -632,7 +641,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -664,22 +673,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E6">
-        <v>31279</v>
+        <v>32279</v>
       </c>
       <c r="F6">
-        <v>95198</v>
+        <v>50119</v>
       </c>
       <c r="G6">
         <v>0.125</v>
@@ -696,22 +705,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E7">
-        <v>32279</v>
+        <v>28974</v>
       </c>
       <c r="F7">
-        <v>50119</v>
+        <v>83580</v>
       </c>
       <c r="G7">
         <v>0.125</v>
@@ -728,22 +737,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>1602</v>
+        <v>2230</v>
       </c>
       <c r="E8">
-        <v>28974</v>
+        <v>32279</v>
       </c>
       <c r="F8">
-        <v>83580</v>
+        <v>50119</v>
       </c>
       <c r="G8">
         <v>0.125</v>
@@ -760,22 +769,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>2040</v>
+        <v>1602</v>
       </c>
       <c r="E9">
-        <v>31279</v>
+        <v>28974</v>
       </c>
       <c r="F9">
-        <v>95198</v>
+        <v>83580</v>
       </c>
       <c r="G9">
         <v>0.125</v>
@@ -792,7 +801,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -824,7 +833,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -856,7 +865,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -888,7 +897,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -920,7 +929,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -952,7 +961,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -984,7 +993,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -996,22 +1005,19 @@
         <v>2230</v>
       </c>
       <c r="E16">
-        <v>30685</v>
+        <v>32279</v>
       </c>
       <c r="F16">
-        <v>48525</v>
+        <v>50119</v>
       </c>
       <c r="G16">
         <v>0.125</v>
       </c>
-      <c r="H16" t="s">
-        <v>31</v>
-      </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="b">
         <v>0</v>
@@ -1019,34 +1025,31 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D17">
-        <v>2230</v>
+        <v>1602</v>
       </c>
       <c r="E17">
-        <v>30685</v>
+        <v>28974</v>
       </c>
       <c r="F17">
-        <v>48525</v>
+        <v>83580</v>
       </c>
       <c r="G17">
         <v>0.125</v>
       </c>
-      <c r="H17" t="s">
-        <v>31</v>
-      </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="b">
         <v>0</v>
@@ -1054,34 +1057,31 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D18">
-        <v>2230</v>
+        <v>2040</v>
       </c>
       <c r="E18">
-        <v>29867</v>
+        <v>31279</v>
       </c>
       <c r="F18">
-        <v>47707</v>
+        <v>95198</v>
       </c>
       <c r="G18">
         <v>0.125</v>
       </c>
-      <c r="H18" t="s">
-        <v>31</v>
-      </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1101,22 +1101,19 @@
         <v>2230</v>
       </c>
       <c r="E19">
-        <v>28867</v>
+        <v>32279</v>
       </c>
       <c r="F19">
-        <v>46707</v>
+        <v>50119</v>
       </c>
       <c r="G19">
         <v>0.125</v>
       </c>
-      <c r="H19" t="s">
-        <v>31</v>
-      </c>
       <c r="I19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="b">
         <v>0</v>
@@ -1124,92 +1121,86 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>2018</v>
+        <v>1602</v>
       </c>
       <c r="E20">
-        <v>19454</v>
+        <v>28974</v>
       </c>
       <c r="F20">
-        <v>71196</v>
+        <v>83580</v>
       </c>
       <c r="G20">
         <v>0.125</v>
       </c>
-      <c r="H20" t="s">
-        <v>31</v>
-      </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
       </c>
       <c r="K20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>1522</v>
+        <v>2040</v>
       </c>
       <c r="E21">
-        <v>16147</v>
+        <v>31279</v>
       </c>
       <c r="F21">
-        <v>56646</v>
+        <v>95198</v>
       </c>
       <c r="G21">
         <v>0.125</v>
       </c>
-      <c r="H21" t="s">
-        <v>31</v>
-      </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
         <v>0</v>
       </c>
       <c r="K21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>1879</v>
+        <v>2230</v>
       </c>
       <c r="E22">
-        <v>18257</v>
+        <v>30685</v>
       </c>
       <c r="F22">
-        <v>67118</v>
+        <v>48525</v>
       </c>
       <c r="G22">
         <v>0.125</v>
@@ -1221,15 +1212,15 @@
         <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1241,10 +1232,10 @@
         <v>2230</v>
       </c>
       <c r="E23">
-        <v>24867</v>
+        <v>30685</v>
       </c>
       <c r="F23">
-        <v>42707</v>
+        <v>48525</v>
       </c>
       <c r="G23">
         <v>0.125</v>
@@ -1264,22 +1255,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>1602</v>
+        <v>2230</v>
       </c>
       <c r="E24">
-        <v>20680</v>
+        <v>29867</v>
       </c>
       <c r="F24">
-        <v>66992</v>
+        <v>47707</v>
       </c>
       <c r="G24">
         <v>0.125</v>
@@ -1299,22 +1290,22 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E25">
-        <v>23600</v>
+        <v>28867</v>
       </c>
       <c r="F25">
-        <v>79840</v>
+        <v>46707</v>
       </c>
       <c r="G25">
         <v>0.125</v>
@@ -1334,7 +1325,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1355,7 +1346,7 @@
         <v>0.125</v>
       </c>
       <c r="H26" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1369,7 +1360,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1390,7 +1381,7 @@
         <v>0.125</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1404,7 +1395,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1425,7 +1416,7 @@
         <v>0.125</v>
       </c>
       <c r="H28" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -1439,7 +1430,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1459,6 +1450,9 @@
       <c r="G29">
         <v>0.125</v>
       </c>
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
@@ -1471,7 +1465,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1483,7 +1477,7 @@
         <v>1602</v>
       </c>
       <c r="E30">
-        <v>21680</v>
+        <v>20680</v>
       </c>
       <c r="F30">
         <v>66992</v>
@@ -1492,7 +1486,7 @@
         <v>0.125</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
@@ -1506,7 +1500,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -1527,7 +1521,7 @@
         <v>0.125</v>
       </c>
       <c r="H31" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1541,7 +1535,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1550,19 +1544,19 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>1928</v>
+        <v>2018</v>
       </c>
       <c r="E32">
-        <v>17342</v>
+        <v>19454</v>
       </c>
       <c r="F32">
-        <v>32766</v>
+        <v>71196</v>
       </c>
       <c r="G32">
         <v>0.125</v>
       </c>
       <c r="H32" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -1576,7 +1570,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1585,19 +1579,19 @@
         <v>6</v>
       </c>
       <c r="D33">
-        <v>1424</v>
+        <v>1522</v>
       </c>
       <c r="E33">
-        <v>14377</v>
+        <v>16147</v>
       </c>
       <c r="F33">
-        <v>25769</v>
+        <v>56646</v>
       </c>
       <c r="G33">
         <v>0.125</v>
       </c>
       <c r="H33" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
@@ -1611,7 +1605,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1620,19 +1614,19 @@
         <v>9</v>
       </c>
       <c r="D34">
-        <v>1782</v>
+        <v>1879</v>
       </c>
       <c r="E34">
-        <v>16483</v>
+        <v>18257</v>
       </c>
       <c r="F34">
-        <v>30739</v>
+        <v>67118</v>
       </c>
       <c r="G34">
         <v>0.125</v>
       </c>
       <c r="H34" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
@@ -1646,7 +1640,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1658,16 +1652,13 @@
         <v>2230</v>
       </c>
       <c r="E35">
-        <v>21968</v>
+        <v>24867</v>
       </c>
       <c r="F35">
-        <v>39808</v>
+        <v>42707</v>
       </c>
       <c r="G35">
         <v>0.125</v>
-      </c>
-      <c r="H35" t="s">
-        <v>21</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -1681,7 +1672,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1693,16 +1684,16 @@
         <v>1602</v>
       </c>
       <c r="E36">
-        <v>18247</v>
+        <v>21680</v>
       </c>
       <c r="F36">
-        <v>31063</v>
+        <v>66992</v>
       </c>
       <c r="G36">
         <v>0.125</v>
       </c>
       <c r="H36" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -1716,7 +1707,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -1728,16 +1719,16 @@
         <v>2040</v>
       </c>
       <c r="E37">
-        <v>21167</v>
+        <v>23600</v>
       </c>
       <c r="F37">
-        <v>37487</v>
+        <v>79840</v>
       </c>
       <c r="G37">
         <v>0.125</v>
       </c>
       <c r="H37" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -1751,7 +1742,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1772,7 +1763,7 @@
         <v>0.125</v>
       </c>
       <c r="H38" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
@@ -1786,7 +1777,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1807,7 +1798,7 @@
         <v>0.125</v>
       </c>
       <c r="H39" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
@@ -1821,7 +1812,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1842,7 +1833,7 @@
         <v>0.125</v>
       </c>
       <c r="H40" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -1856,7 +1847,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1868,16 +1859,16 @@
         <v>2230</v>
       </c>
       <c r="E41">
-        <v>20500</v>
+        <v>21968</v>
       </c>
       <c r="F41">
-        <v>38340</v>
+        <v>39808</v>
       </c>
       <c r="G41">
         <v>0.125</v>
       </c>
       <c r="H41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I41" t="b">
         <v>0</v>
@@ -1891,7 +1882,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -1903,16 +1894,16 @@
         <v>1602</v>
       </c>
       <c r="E42">
-        <v>16806</v>
+        <v>18247</v>
       </c>
       <c r="F42">
-        <v>29622</v>
+        <v>31063</v>
       </c>
       <c r="G42">
         <v>0.125</v>
       </c>
       <c r="H42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
@@ -1926,7 +1917,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -1938,16 +1929,16 @@
         <v>2040</v>
       </c>
       <c r="E43">
-        <v>19383</v>
+        <v>21167</v>
       </c>
       <c r="F43">
-        <v>35703</v>
+        <v>37487</v>
       </c>
       <c r="G43">
         <v>0.125</v>
       </c>
       <c r="H43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I43" t="b">
         <v>0</v>
@@ -1961,7 +1952,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1982,7 +1973,7 @@
         <v>0.125</v>
       </c>
       <c r="H44" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
@@ -1996,7 +1987,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -2017,7 +2008,7 @@
         <v>0.125</v>
       </c>
       <c r="H45" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
@@ -2031,7 +2022,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -2052,7 +2043,7 @@
         <v>0.125</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I46" t="b">
         <v>0</v>
@@ -2066,7 +2057,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2087,7 +2078,7 @@
         <v>0.125</v>
       </c>
       <c r="H47" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
@@ -2101,7 +2092,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -2122,7 +2113,7 @@
         <v>0.125</v>
       </c>
       <c r="H48" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2136,7 +2127,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -2157,13 +2148,13 @@
         <v>0.125</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
       <c r="J49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" t="b">
         <v>0</v>
@@ -2171,7 +2162,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2180,7 +2171,7 @@
         <v>4</v>
       </c>
       <c r="D50">
-        <v>1925</v>
+        <v>1928</v>
       </c>
       <c r="E50">
         <v>17342</v>
@@ -2192,7 +2183,7 @@
         <v>0.125</v>
       </c>
       <c r="H50" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
@@ -2206,7 +2197,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -2227,7 +2218,7 @@
         <v>0.125</v>
       </c>
       <c r="H51" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
@@ -2241,7 +2232,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -2262,7 +2253,7 @@
         <v>0.125</v>
       </c>
       <c r="H52" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I52" t="b">
         <v>0</v>
@@ -2276,7 +2267,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2285,30 +2276,33 @@
         <v>4</v>
       </c>
       <c r="D53">
-        <v>1710</v>
+        <v>2230</v>
       </c>
       <c r="E53">
-        <v>16059</v>
+        <v>20500</v>
       </c>
       <c r="F53">
-        <v>29739</v>
+        <v>38340</v>
+      </c>
+      <c r="G53">
+        <v>0.125</v>
       </c>
       <c r="H53" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I53" t="b">
         <v>0</v>
       </c>
       <c r="J53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -2317,30 +2311,33 @@
         <v>6</v>
       </c>
       <c r="D54">
-        <v>1245</v>
+        <v>1602</v>
       </c>
       <c r="E54">
-        <v>13324</v>
+        <v>16806</v>
       </c>
       <c r="F54">
-        <v>23284</v>
+        <v>29622</v>
+      </c>
+      <c r="G54">
+        <v>0.125</v>
       </c>
       <c r="H54" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I54" t="b">
         <v>0</v>
       </c>
       <c r="J54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -2349,16 +2346,19 @@
         <v>9</v>
       </c>
       <c r="D55">
-        <v>1573</v>
+        <v>2040</v>
       </c>
       <c r="E55">
-        <v>15253</v>
+        <v>19383</v>
       </c>
       <c r="F55">
-        <v>27837</v>
+        <v>35703</v>
+      </c>
+      <c r="G55">
+        <v>0.125</v>
       </c>
       <c r="H55" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I55" t="b">
         <v>0</v>
@@ -2367,12 +2367,12 @@
         <v>0</v>
       </c>
       <c r="K55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2381,13 +2381,16 @@
         <v>4</v>
       </c>
       <c r="D56">
-        <v>1608</v>
+        <v>1925</v>
       </c>
       <c r="E56">
-        <v>15459</v>
+        <v>17342</v>
       </c>
       <c r="F56">
-        <v>28323</v>
+        <v>32766</v>
+      </c>
+      <c r="G56">
+        <v>0.125</v>
       </c>
       <c r="H56" t="s">
         <v>34</v>
@@ -2404,7 +2407,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -2413,13 +2416,16 @@
         <v>6</v>
       </c>
       <c r="D57">
-        <v>1155</v>
+        <v>1424</v>
       </c>
       <c r="E57">
-        <v>12795</v>
+        <v>14377</v>
       </c>
       <c r="F57">
-        <v>22035</v>
+        <v>25769</v>
+      </c>
+      <c r="G57">
+        <v>0.125</v>
       </c>
       <c r="H57" t="s">
         <v>34</v>
@@ -2436,7 +2442,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -2445,13 +2451,16 @@
         <v>9</v>
       </c>
       <c r="D58">
-        <v>1471</v>
+        <v>1782</v>
       </c>
       <c r="E58">
-        <v>14653</v>
+        <v>16483</v>
       </c>
       <c r="F58">
-        <v>26421</v>
+        <v>30739</v>
+      </c>
+      <c r="G58">
+        <v>0.125</v>
       </c>
       <c r="H58" t="s">
         <v>34</v>
@@ -2466,11 +2475,203 @@
         <v>1</v>
       </c>
     </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>1710</v>
+      </c>
+      <c r="E59">
+        <v>16059</v>
+      </c>
+      <c r="F59">
+        <v>29739</v>
+      </c>
+      <c r="H59" t="s">
+        <v>34</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>1245</v>
+      </c>
+      <c r="E60">
+        <v>13324</v>
+      </c>
+      <c r="F60">
+        <v>23284</v>
+      </c>
+      <c r="H60" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61">
+        <v>1573</v>
+      </c>
+      <c r="E61">
+        <v>15253</v>
+      </c>
+      <c r="F61">
+        <v>27837</v>
+      </c>
+      <c r="H61" t="s">
+        <v>34</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>1608</v>
+      </c>
+      <c r="E62">
+        <v>15459</v>
+      </c>
+      <c r="F62">
+        <v>28323</v>
+      </c>
+      <c r="H62" t="s">
+        <v>34</v>
+      </c>
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63">
+        <v>1155</v>
+      </c>
+      <c r="E63">
+        <v>12795</v>
+      </c>
+      <c r="F63">
+        <v>22035</v>
+      </c>
+      <c r="H63" t="s">
+        <v>34</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64">
+        <v>1471</v>
+      </c>
+      <c r="E64">
+        <v>14653</v>
+      </c>
+      <c r="F64">
+        <v>26421</v>
+      </c>
+      <c r="H64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:K49">
-    <sortCondition descending="1" ref="A2:A49"/>
-    <sortCondition ref="I2:I49"/>
-    <sortCondition ref="J2:J49"/>
+  <sortState ref="A8:K55">
+    <sortCondition descending="1" ref="A8:A55"/>
+    <sortCondition ref="I8:I55"/>
+    <sortCondition ref="J8:J55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update data post-Budget 2019
</commit_message>
<xml_diff>
--- a/data-raw/SAPTO-rates.xlsx
+++ b/data-raw/SAPTO-rates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughp\Documents\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcowgill/Dropbox (Personal)/R/packages/hughparsonage/grattan/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9416EE97-0AE2-D34D-A89D-78B88B9D13A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="41">
   <si>
     <t>fy_year</t>
   </si>
@@ -144,12 +145,15 @@
   </si>
   <si>
     <t>2019-20</t>
+  </si>
+  <si>
+    <t>2020-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,21 +498,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="74" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,9 +547,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -575,9 +579,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -607,9 +611,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -639,9 +643,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -671,9 +675,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -703,9 +707,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -735,9 +739,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -767,9 +771,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -799,9 +803,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -831,9 +835,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -863,89 +867,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>2230</v>
+      </c>
+      <c r="E12">
+        <v>32279</v>
+      </c>
+      <c r="F12">
+        <v>50119</v>
+      </c>
+      <c r="G12">
+        <v>0.125</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>1602</v>
+      </c>
+      <c r="E13">
+        <v>28974</v>
+      </c>
+      <c r="F13">
+        <v>83580</v>
+      </c>
+      <c r="G13">
+        <v>0.125</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <v>2040</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <v>31279</v>
       </c>
-      <c r="F12">
+      <c r="F14">
         <v>95198</v>
       </c>
-      <c r="G12">
-        <v>0.125</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>2230</v>
-      </c>
-      <c r="E13">
-        <v>32279</v>
-      </c>
-      <c r="F13">
-        <v>50119</v>
-      </c>
-      <c r="G13">
-        <v>0.125</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>1602</v>
-      </c>
-      <c r="E14">
-        <v>28974</v>
-      </c>
-      <c r="F14">
-        <v>83580</v>
-      </c>
       <c r="G14">
         <v>0.125</v>
       </c>
@@ -959,89 +963,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>2230</v>
+      </c>
+      <c r="E15">
+        <v>32279</v>
+      </c>
+      <c r="F15">
+        <v>50119</v>
+      </c>
+      <c r="G15">
+        <v>0.125</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>1602</v>
+      </c>
+      <c r="E16">
+        <v>28974</v>
+      </c>
+      <c r="F16">
+        <v>83580</v>
+      </c>
+      <c r="G16">
+        <v>0.125</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>2040</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>31279</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>95198</v>
       </c>
-      <c r="G15">
-        <v>0.125</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>2230</v>
-      </c>
-      <c r="E16">
-        <v>32279</v>
-      </c>
-      <c r="F16">
-        <v>50119</v>
-      </c>
-      <c r="G16">
-        <v>0.125</v>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>1602</v>
-      </c>
-      <c r="E17">
-        <v>28974</v>
-      </c>
-      <c r="F17">
-        <v>83580</v>
-      </c>
       <c r="G17">
         <v>0.125</v>
       </c>
@@ -1055,207 +1059,201 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>2230</v>
+      </c>
+      <c r="E18">
+        <v>32279</v>
+      </c>
+      <c r="F18">
+        <v>50119</v>
+      </c>
+      <c r="G18">
+        <v>0.125</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1602</v>
+      </c>
+      <c r="E19">
+        <v>28974</v>
+      </c>
+      <c r="F19">
+        <v>83580</v>
+      </c>
+      <c r="G19">
+        <v>0.125</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>2040</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <v>31279</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <v>95198</v>
       </c>
-      <c r="G18">
-        <v>0.125</v>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="G20">
+        <v>0.125</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>2230</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>32279</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>50119</v>
       </c>
-      <c r="G19">
-        <v>0.125</v>
-      </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20">
+      <c r="G21">
+        <v>0.125</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>1602</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <v>28974</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>83580</v>
       </c>
-      <c r="G20">
-        <v>0.125</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21">
+      <c r="G22">
+        <v>0.125</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>2040</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <v>31279</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>95198</v>
       </c>
-      <c r="G21">
-        <v>0.125</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G23">
+        <v>0.125</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>30</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>2230</v>
-      </c>
-      <c r="E22">
-        <v>30685</v>
-      </c>
-      <c r="F22">
-        <v>48525</v>
-      </c>
-      <c r="G22">
-        <v>0.125</v>
-      </c>
-      <c r="H22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>2230</v>
-      </c>
-      <c r="E23">
-        <v>30685</v>
-      </c>
-      <c r="F23">
-        <v>48525</v>
-      </c>
-      <c r="G23">
-        <v>0.125</v>
-      </c>
-      <c r="H23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1267,10 +1265,10 @@
         <v>2230</v>
       </c>
       <c r="E24">
-        <v>29867</v>
+        <v>30685</v>
       </c>
       <c r="F24">
-        <v>47707</v>
+        <v>48525</v>
       </c>
       <c r="G24">
         <v>0.125</v>
@@ -1288,9 +1286,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1302,10 +1300,10 @@
         <v>2230</v>
       </c>
       <c r="E25">
-        <v>28867</v>
+        <v>30685</v>
       </c>
       <c r="F25">
-        <v>46707</v>
+        <v>48525</v>
       </c>
       <c r="G25">
         <v>0.125</v>
@@ -1323,9 +1321,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1334,13 +1332,13 @@
         <v>4</v>
       </c>
       <c r="D26">
-        <v>2018</v>
+        <v>2230</v>
       </c>
       <c r="E26">
-        <v>19454</v>
+        <v>29867</v>
       </c>
       <c r="F26">
-        <v>71196</v>
+        <v>47707</v>
       </c>
       <c r="G26">
         <v>0.125</v>
@@ -1352,30 +1350,30 @@
         <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>1522</v>
+        <v>2230</v>
       </c>
       <c r="E27">
-        <v>16147</v>
+        <v>28867</v>
       </c>
       <c r="F27">
-        <v>56646</v>
+        <v>46707</v>
       </c>
       <c r="G27">
         <v>0.125</v>
@@ -1387,30 +1385,30 @@
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D28">
-        <v>1879</v>
+        <v>2018</v>
       </c>
       <c r="E28">
-        <v>18257</v>
+        <v>19454</v>
       </c>
       <c r="F28">
-        <v>67118</v>
+        <v>71196</v>
       </c>
       <c r="G28">
         <v>0.125</v>
@@ -1428,24 +1426,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>2230</v>
+        <v>1522</v>
       </c>
       <c r="E29">
-        <v>24867</v>
+        <v>16147</v>
       </c>
       <c r="F29">
-        <v>42707</v>
+        <v>56646</v>
       </c>
       <c r="G29">
         <v>0.125</v>
@@ -1457,30 +1455,30 @@
         <v>0</v>
       </c>
       <c r="J29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D30">
-        <v>1602</v>
+        <v>1879</v>
       </c>
       <c r="E30">
-        <v>20680</v>
+        <v>18257</v>
       </c>
       <c r="F30">
-        <v>66992</v>
+        <v>67118</v>
       </c>
       <c r="G30">
         <v>0.125</v>
@@ -1492,30 +1490,30 @@
         <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E31">
-        <v>23600</v>
+        <v>24867</v>
       </c>
       <c r="F31">
-        <v>79840</v>
+        <v>42707</v>
       </c>
       <c r="G31">
         <v>0.125</v>
@@ -1533,94 +1531,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>2018</v>
+        <v>1602</v>
       </c>
       <c r="E32">
-        <v>19454</v>
+        <v>20680</v>
       </c>
       <c r="F32">
-        <v>71196</v>
+        <v>66992</v>
       </c>
       <c r="G32">
         <v>0.125</v>
       </c>
       <c r="H32" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D33">
-        <v>1522</v>
+        <v>2040</v>
       </c>
       <c r="E33">
-        <v>16147</v>
+        <v>23600</v>
       </c>
       <c r="F33">
-        <v>56646</v>
+        <v>79840</v>
       </c>
       <c r="G33">
         <v>0.125</v>
       </c>
       <c r="H33" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>24</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>1879</v>
+        <v>2018</v>
       </c>
       <c r="E34">
-        <v>18257</v>
+        <v>19454</v>
       </c>
       <c r="F34">
-        <v>67118</v>
+        <v>71196</v>
       </c>
       <c r="G34">
         <v>0.125</v>
@@ -1638,56 +1636,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>24</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D35">
-        <v>2230</v>
+        <v>1522</v>
       </c>
       <c r="E35">
-        <v>24867</v>
+        <v>16147</v>
       </c>
       <c r="F35">
-        <v>42707</v>
+        <v>56646</v>
       </c>
       <c r="G35">
         <v>0.125</v>
       </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
       <c r="I35" t="b">
         <v>0</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D36">
-        <v>1602</v>
+        <v>1879</v>
       </c>
       <c r="E36">
-        <v>21680</v>
+        <v>18257</v>
       </c>
       <c r="F36">
-        <v>66992</v>
+        <v>67118</v>
       </c>
       <c r="G36">
         <v>0.125</v>
@@ -1699,135 +1700,132 @@
         <v>0</v>
       </c>
       <c r="J36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>24</v>
       </c>
       <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>2230</v>
+      </c>
+      <c r="E37">
+        <v>24867</v>
+      </c>
+      <c r="F37">
+        <v>42707</v>
+      </c>
+      <c r="G37">
+        <v>0.125</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>1602</v>
+      </c>
+      <c r="E38">
+        <v>21680</v>
+      </c>
+      <c r="F38">
+        <v>66992</v>
+      </c>
+      <c r="G38">
+        <v>0.125</v>
+      </c>
+      <c r="H38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39">
         <v>3</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>9</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>2040</v>
       </c>
-      <c r="E37">
+      <c r="E39">
         <v>23600</v>
       </c>
-      <c r="F37">
+      <c r="F39">
         <v>79840</v>
       </c>
-      <c r="G37">
-        <v>0.125</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="G39">
+        <v>0.125</v>
+      </c>
+      <c r="H39" t="s">
         <v>25</v>
       </c>
-      <c r="I37" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38">
-        <v>1928</v>
-      </c>
-      <c r="E38">
-        <v>17342</v>
-      </c>
-      <c r="F38">
-        <v>32766</v>
-      </c>
-      <c r="G38">
-        <v>0.125</v>
-      </c>
-      <c r="H38" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
-        <v>1424</v>
-      </c>
-      <c r="E39">
-        <v>14377</v>
-      </c>
-      <c r="F39">
-        <v>25769</v>
-      </c>
-      <c r="G39">
-        <v>0.125</v>
-      </c>
-      <c r="H39" t="s">
-        <v>21</v>
-      </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D40">
-        <v>1782</v>
+        <v>1928</v>
       </c>
       <c r="E40">
-        <v>16483</v>
+        <v>17342</v>
       </c>
       <c r="F40">
-        <v>30739</v>
+        <v>32766</v>
       </c>
       <c r="G40">
         <v>0.125</v>
@@ -1845,24 +1843,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D41">
-        <v>2230</v>
+        <v>1424</v>
       </c>
       <c r="E41">
-        <v>21968</v>
+        <v>14377</v>
       </c>
       <c r="F41">
-        <v>39808</v>
+        <v>25769</v>
       </c>
       <c r="G41">
         <v>0.125</v>
@@ -1874,30 +1872,30 @@
         <v>0</v>
       </c>
       <c r="J41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>22</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D42">
-        <v>1602</v>
+        <v>1782</v>
       </c>
       <c r="E42">
-        <v>18247</v>
+        <v>16483</v>
       </c>
       <c r="F42">
-        <v>31063</v>
+        <v>30739</v>
       </c>
       <c r="G42">
         <v>0.125</v>
@@ -1909,30 +1907,30 @@
         <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>22</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E43">
-        <v>21167</v>
+        <v>21968</v>
       </c>
       <c r="F43">
-        <v>37487</v>
+        <v>39808</v>
       </c>
       <c r="G43">
         <v>0.125</v>
@@ -1950,94 +1948,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D44">
-        <v>1928</v>
+        <v>1602</v>
       </c>
       <c r="E44">
-        <v>17342</v>
+        <v>18247</v>
       </c>
       <c r="F44">
-        <v>32766</v>
+        <v>31063</v>
       </c>
       <c r="G44">
         <v>0.125</v>
       </c>
       <c r="H44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D45">
-        <v>1424</v>
+        <v>2040</v>
       </c>
       <c r="E45">
-        <v>14377</v>
+        <v>21167</v>
       </c>
       <c r="F45">
-        <v>25769</v>
+        <v>37487</v>
       </c>
       <c r="G45">
         <v>0.125</v>
       </c>
       <c r="H45" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>20</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D46">
-        <v>1782</v>
+        <v>1928</v>
       </c>
       <c r="E46">
-        <v>16483</v>
+        <v>17342</v>
       </c>
       <c r="F46">
-        <v>30739</v>
+        <v>32766</v>
       </c>
       <c r="G46">
         <v>0.125</v>
@@ -2055,24 +2053,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D47">
-        <v>2230</v>
+        <v>1424</v>
       </c>
       <c r="E47">
-        <v>20500</v>
+        <v>14377</v>
       </c>
       <c r="F47">
-        <v>38340</v>
+        <v>25769</v>
       </c>
       <c r="G47">
         <v>0.125</v>
@@ -2084,30 +2082,30 @@
         <v>0</v>
       </c>
       <c r="J47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>20</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D48">
-        <v>1602</v>
+        <v>1782</v>
       </c>
       <c r="E48">
-        <v>16806</v>
+        <v>16483</v>
       </c>
       <c r="F48">
-        <v>29622</v>
+        <v>30739</v>
       </c>
       <c r="G48">
         <v>0.125</v>
@@ -2119,30 +2117,30 @@
         <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D49">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E49">
-        <v>19383</v>
+        <v>20500</v>
       </c>
       <c r="F49">
-        <v>35703</v>
+        <v>38340</v>
       </c>
       <c r="G49">
         <v>0.125</v>
@@ -2160,94 +2158,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>1928</v>
+        <v>1602</v>
       </c>
       <c r="E50">
-        <v>17342</v>
+        <v>16806</v>
       </c>
       <c r="F50">
-        <v>32766</v>
+        <v>29622</v>
       </c>
       <c r="G50">
         <v>0.125</v>
       </c>
       <c r="H50" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I50" t="b">
         <v>0</v>
       </c>
       <c r="J50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D51">
-        <v>1424</v>
+        <v>2040</v>
       </c>
       <c r="E51">
-        <v>14377</v>
+        <v>19383</v>
       </c>
       <c r="F51">
-        <v>25769</v>
+        <v>35703</v>
       </c>
       <c r="G51">
         <v>0.125</v>
       </c>
       <c r="H51" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
       </c>
       <c r="J51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>14</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D52">
-        <v>1782</v>
+        <v>1928</v>
       </c>
       <c r="E52">
-        <v>16483</v>
+        <v>17342</v>
       </c>
       <c r="F52">
-        <v>30739</v>
+        <v>32766</v>
       </c>
       <c r="G52">
         <v>0.125</v>
@@ -2265,24 +2263,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>14</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D53">
-        <v>2230</v>
+        <v>1424</v>
       </c>
       <c r="E53">
-        <v>20500</v>
+        <v>14377</v>
       </c>
       <c r="F53">
-        <v>38340</v>
+        <v>25769</v>
       </c>
       <c r="G53">
         <v>0.125</v>
@@ -2294,30 +2292,30 @@
         <v>0</v>
       </c>
       <c r="J53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D54">
-        <v>1602</v>
+        <v>1782</v>
       </c>
       <c r="E54">
-        <v>16806</v>
+        <v>16483</v>
       </c>
       <c r="F54">
-        <v>29622</v>
+        <v>30739</v>
       </c>
       <c r="G54">
         <v>0.125</v>
@@ -2329,30 +2327,30 @@
         <v>0</v>
       </c>
       <c r="J54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>14</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D55">
-        <v>2040</v>
+        <v>2230</v>
       </c>
       <c r="E55">
-        <v>19383</v>
+        <v>20500</v>
       </c>
       <c r="F55">
-        <v>35703</v>
+        <v>38340</v>
       </c>
       <c r="G55">
         <v>0.125</v>
@@ -2364,71 +2362,71 @@
         <v>0</v>
       </c>
       <c r="J55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D56">
-        <v>1925</v>
+        <v>1602</v>
       </c>
       <c r="E56">
-        <v>17342</v>
+        <v>16806</v>
       </c>
       <c r="F56">
-        <v>32766</v>
+        <v>29622</v>
       </c>
       <c r="G56">
         <v>0.125</v>
       </c>
       <c r="H56" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I56" t="b">
         <v>0</v>
       </c>
       <c r="J56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D57">
-        <v>1424</v>
+        <v>2040</v>
       </c>
       <c r="E57">
-        <v>14377</v>
+        <v>19383</v>
       </c>
       <c r="F57">
-        <v>25769</v>
+        <v>35703</v>
       </c>
       <c r="G57">
         <v>0.125</v>
       </c>
       <c r="H57" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I57" t="b">
         <v>0</v>
@@ -2437,27 +2435,27 @@
         <v>0</v>
       </c>
       <c r="K57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>33</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D58">
-        <v>1782</v>
+        <v>1925</v>
       </c>
       <c r="E58">
-        <v>16483</v>
+        <v>17342</v>
       </c>
       <c r="F58">
-        <v>30739</v>
+        <v>32766</v>
       </c>
       <c r="G58">
         <v>0.125</v>
@@ -2475,24 +2473,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D59">
-        <v>1710</v>
+        <v>1424</v>
       </c>
       <c r="E59">
-        <v>16059</v>
+        <v>14377</v>
       </c>
       <c r="F59">
-        <v>29739</v>
+        <v>25769</v>
+      </c>
+      <c r="G59">
+        <v>0.125</v>
       </c>
       <c r="H59" t="s">
         <v>34</v>
@@ -2507,24 +2508,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D60">
-        <v>1245</v>
+        <v>1782</v>
       </c>
       <c r="E60">
-        <v>13324</v>
+        <v>16483</v>
       </c>
       <c r="F60">
-        <v>23284</v>
+        <v>30739</v>
+      </c>
+      <c r="G60">
+        <v>0.125</v>
       </c>
       <c r="H60" t="s">
         <v>34</v>
@@ -2539,24 +2543,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>35</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D61">
-        <v>1573</v>
+        <v>1710</v>
       </c>
       <c r="E61">
-        <v>15253</v>
+        <v>16059</v>
       </c>
       <c r="F61">
-        <v>27837</v>
+        <v>29739</v>
       </c>
       <c r="H61" t="s">
         <v>34</v>
@@ -2571,24 +2575,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D62">
-        <v>1608</v>
+        <v>1245</v>
       </c>
       <c r="E62">
-        <v>15459</v>
+        <v>13324</v>
       </c>
       <c r="F62">
-        <v>28323</v>
+        <v>23284</v>
       </c>
       <c r="H62" t="s">
         <v>34</v>
@@ -2603,24 +2607,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D63">
-        <v>1155</v>
+        <v>1573</v>
       </c>
       <c r="E63">
-        <v>12795</v>
+        <v>15253</v>
       </c>
       <c r="F63">
-        <v>22035</v>
+        <v>27837</v>
       </c>
       <c r="H63" t="s">
         <v>34</v>
@@ -2635,24 +2639,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>36</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D64">
-        <v>1471</v>
+        <v>1608</v>
       </c>
       <c r="E64">
-        <v>14653</v>
+        <v>15459</v>
       </c>
       <c r="F64">
-        <v>26421</v>
+        <v>28323</v>
       </c>
       <c r="H64" t="s">
         <v>34</v>
@@ -2667,11 +2671,75 @@
         <v>1</v>
       </c>
     </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>1155</v>
+      </c>
+      <c r="E65">
+        <v>12795</v>
+      </c>
+      <c r="F65">
+        <v>22035</v>
+      </c>
+      <c r="H65" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66">
+        <v>1471</v>
+      </c>
+      <c r="E66">
+        <v>14653</v>
+      </c>
+      <c r="F66">
+        <v>26421</v>
+      </c>
+      <c r="H66" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A8:K55">
-    <sortCondition descending="1" ref="A8:A55"/>
-    <sortCondition ref="I8:I55"/>
-    <sortCondition ref="J8:J55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:K57">
+    <sortCondition descending="1" ref="A10:A57"/>
+    <sortCondition ref="I10:I57"/>
+    <sortCondition ref="J10:J57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>